<commit_message>
Ajout des liens pour les réseaux sociaux
</commit_message>
<xml_diff>
--- a/Doc/P4_04_rapport.xlsx
+++ b/Doc/P4_04_rapport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISMAIL\Documents\Starting website\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISMAIL\Documents\La chouette agence\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E452256F-4EF3-44A7-B9A6-93D73D2D5D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA318A98-3D0A-48AA-8761-9DF1F6A552FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inspecteur" sheetId="1" r:id="rId1"/>
@@ -84,6 +84,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -322,12 +323,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,6 +331,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,22 +826,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>145227</xdr:rowOff>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>411954</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:colOff>336049</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A3BFEB0-6DFF-454B-9CDD-466AF60824D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A08F758F-EA8B-4D8E-97CA-B8B6C983C171}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -862,8 +863,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="190500" y="5803077"/>
-          <a:ext cx="9622629" cy="4217222"/>
+          <a:off x="285750" y="5800724"/>
+          <a:ext cx="9451474" cy="3962401"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1143,7 +1144,7 @@
   </sheetPr>
   <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1153,7 +1154,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1"/>
@@ -1190,12 +1191,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:5" ht="35.25" x14ac:dyDescent="0.2">
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="21" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="5:5" ht="35.25" x14ac:dyDescent="0.2">
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1324,7 +1325,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="13" t="s">
@@ -1332,7 +1333,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="14" t="s">
         <v>5</v>
       </c>
@@ -1407,7 +1408,7 @@
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B55" s="13" t="s">
@@ -1415,7 +1416,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
+      <c r="A56" s="23"/>
       <c r="B56" s="14" t="s">
         <v>5</v>
       </c>
@@ -1448,8 +1449,8 @@
   </sheetPr>
   <dimension ref="D2:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1459,12 +1460,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:4" ht="35.25" x14ac:dyDescent="0.5">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:5" ht="35.25" x14ac:dyDescent="0.5">
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="19" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>